<commit_message>
New methodology with proper results and improved accuracy
</commit_message>
<xml_diff>
--- a/dyes_DFT_PBE_dataset.xlsx
+++ b/dyes_DFT_PBE_dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,592 +530,851 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>12a</t>
+          <t>10c</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-4.636</v>
+        <v>-4.684</v>
       </c>
       <c r="C3" t="n">
-        <v>-3.698</v>
+        <v>-3.682</v>
       </c>
       <c r="D3" t="n">
-        <v>27.223</v>
+        <v>20.2171</v>
       </c>
       <c r="E3" t="n">
-        <v>-2857.553234</v>
+        <v>-2677.852681</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.203</v>
+        <v>-1.105</v>
       </c>
       <c r="G3" t="n">
-        <v>596.582989</v>
+        <v>763.2236789999999</v>
       </c>
       <c r="H3" t="n">
-        <v>652.896473</v>
+        <v>840.423948</v>
       </c>
       <c r="I3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>592</v>
+        <v>558</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9993840000000001</v>
+        <v>1.084045</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20a</t>
+          <t>10d</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-4.651</v>
+        <v>-4.615</v>
       </c>
       <c r="C4" t="n">
-        <v>-3.727</v>
+        <v>-3.677</v>
       </c>
       <c r="D4" t="n">
-        <v>26.3601</v>
+        <v>18.4425</v>
       </c>
       <c r="E4" t="n">
-        <v>-2216.160004</v>
+        <v>-2523.17176</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.214</v>
+        <v>-1.031</v>
       </c>
       <c r="G4" t="n">
-        <v>608.199673</v>
+        <v>697.440336</v>
       </c>
       <c r="H4" t="n">
-        <v>664.73637</v>
+        <v>770.669635</v>
       </c>
       <c r="I4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>561</v>
+        <v>510</v>
       </c>
       <c r="K4" t="n">
-        <v>1.05693</v>
+        <v>0.547976</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>21a</t>
+          <t>12a</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-4.561</v>
+        <v>-4.636</v>
       </c>
       <c r="C5" t="n">
-        <v>-3.715</v>
+        <v>-3.698</v>
       </c>
       <c r="D5" t="n">
-        <v>23.7772</v>
+        <v>27.223</v>
       </c>
       <c r="E5" t="n">
-        <v>-2767.699232</v>
+        <v>-2857.553234</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.31</v>
+        <v>-1.203</v>
       </c>
       <c r="G5" t="n">
-        <v>678.557941</v>
+        <v>596.582989</v>
       </c>
       <c r="H5" t="n">
-        <v>748.458472</v>
+        <v>652.896473</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="J5" t="n">
-        <v>637</v>
+        <v>592</v>
       </c>
       <c r="K5" t="n">
-        <v>0.705128</v>
+        <v>0.9993840000000001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>D1</t>
+          <t>12b</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-5.195</v>
+        <v>-4.624</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.63</v>
+        <v>-3.677</v>
       </c>
       <c r="D6" t="n">
-        <v>6.5592</v>
+        <v>14.9789</v>
       </c>
       <c r="E6" t="n">
-        <v>-1393.134805</v>
+        <v>-3498.950342</v>
       </c>
       <c r="F6" t="n">
-        <v>-1.184</v>
+        <v>-0.944</v>
       </c>
       <c r="G6" t="n">
-        <v>387.3409</v>
+        <v>582.016851</v>
       </c>
       <c r="H6" t="n">
-        <v>412.951353</v>
+        <v>641.354295</v>
       </c>
       <c r="I6" t="n">
         <v>-0</v>
       </c>
       <c r="J6" t="n">
-        <v>408</v>
+        <v>528</v>
       </c>
       <c r="K6" t="n">
-        <v>0.17197</v>
+        <v>0.889745</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>D2</t>
+          <t>19a</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-5.163</v>
+        <v>-4.71</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.589</v>
+        <v>-3.587</v>
       </c>
       <c r="D7" t="n">
-        <v>6.8226</v>
+        <v>16.8789</v>
       </c>
       <c r="E7" t="n">
-        <v>-1278.684862</v>
+        <v>-1985.333899</v>
       </c>
       <c r="F7" t="n">
-        <v>-1.054</v>
+        <v>-1.026</v>
       </c>
       <c r="G7" t="n">
-        <v>354.439145</v>
+        <v>544.1936920000001</v>
       </c>
       <c r="H7" t="n">
-        <v>380.068067</v>
+        <v>582.522059</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="J7" t="n">
-        <v>409</v>
+        <v>530</v>
       </c>
       <c r="K7" t="n">
-        <v>0.234811</v>
+        <v>0.7176399999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>D3</t>
+          <t>20a</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-5.271</v>
+        <v>-4.651</v>
       </c>
       <c r="C8" t="n">
-        <v>-2.633</v>
+        <v>-3.727</v>
       </c>
       <c r="D8" t="n">
-        <v>3.3748</v>
+        <v>26.3601</v>
       </c>
       <c r="E8" t="n">
-        <v>-1444.874262</v>
+        <v>-2216.160004</v>
       </c>
       <c r="F8" t="n">
-        <v>-1.061</v>
+        <v>-1.214</v>
       </c>
       <c r="G8" t="n">
-        <v>346.581779</v>
+        <v>608.199673</v>
       </c>
       <c r="H8" t="n">
-        <v>402.922143</v>
+        <v>664.73637</v>
       </c>
       <c r="I8" t="n">
         <v>-0</v>
       </c>
       <c r="J8" t="n">
-        <v>359</v>
+        <v>561</v>
       </c>
       <c r="K8" t="n">
-        <v>0.109098</v>
+        <v>1.05693</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DPAA</t>
+          <t>21a</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-4.862</v>
+        <v>-4.561</v>
       </c>
       <c r="C9" t="n">
-        <v>-2.735</v>
+        <v>-3.715</v>
       </c>
       <c r="D9" t="n">
-        <v>5.8789</v>
+        <v>23.7772</v>
       </c>
       <c r="E9" t="n">
-        <v>-3704.69389</v>
+        <v>-2767.699232</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.6850000000000001</v>
+        <v>-1.31</v>
       </c>
       <c r="G9" t="n">
-        <v>389.939641</v>
+        <v>678.557941</v>
       </c>
       <c r="H9" t="n">
-        <v>426.054576</v>
+        <v>748.458472</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>474</v>
+        <v>637</v>
       </c>
       <c r="K9" t="n">
-        <v>0.499187</v>
+        <v>0.705128</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DPACA</t>
+          <t>22a</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-5.095</v>
+        <v>-4.558</v>
       </c>
       <c r="C10" t="n">
-        <v>-3.249</v>
+        <v>-3.68</v>
       </c>
       <c r="D10" t="n">
-        <v>7.7768</v>
+        <v>21.2796</v>
       </c>
       <c r="E10" t="n">
-        <v>-3796.874182</v>
+        <v>-3319.255172</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.8159999999999999</v>
+        <v>-1.171</v>
       </c>
       <c r="G10" t="n">
-        <v>412.305213</v>
+        <v>747.679262</v>
       </c>
       <c r="H10" t="n">
-        <v>452.543801</v>
+        <v>828.789887</v>
       </c>
       <c r="I10" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>519</v>
+        <v>682</v>
       </c>
       <c r="K10" t="n">
-        <v>0.533851</v>
+        <v>1.470767</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Phenothiazine1</t>
+          <t>D1</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-4.935</v>
+        <v>-5.195</v>
       </c>
       <c r="C11" t="n">
-        <v>-3.333</v>
+        <v>-2.63</v>
       </c>
       <c r="D11" t="n">
-        <v>9.0352</v>
+        <v>6.5592</v>
       </c>
       <c r="E11" t="n">
-        <v>-1351.57215</v>
+        <v>-1393.134805</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.765</v>
+        <v>-1.184</v>
       </c>
       <c r="G11" t="n">
-        <v>330.452395</v>
+        <v>387.3409</v>
       </c>
       <c r="H11" t="n">
-        <v>349.95115</v>
+        <v>412.951353</v>
       </c>
       <c r="I11" t="n">
         <v>-0</v>
       </c>
       <c r="J11" t="n">
-        <v>343</v>
+        <v>408</v>
       </c>
       <c r="K11" t="n">
-        <v>0.288586</v>
+        <v>0.17197</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Phenothiazine2</t>
+          <t>D2</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-4.818</v>
+        <v>-5.163</v>
       </c>
       <c r="C12" t="n">
-        <v>-2.806</v>
+        <v>-2.589</v>
       </c>
       <c r="D12" t="n">
-        <v>7.2013</v>
+        <v>6.8226</v>
       </c>
       <c r="E12" t="n">
-        <v>-1259.394134</v>
+        <v>-1278.684862</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.631</v>
+        <v>-1.054</v>
       </c>
       <c r="G12" t="n">
-        <v>311.25871</v>
+        <v>354.439145</v>
       </c>
       <c r="H12" t="n">
-        <v>327.396927</v>
+        <v>380.068067</v>
       </c>
       <c r="I12" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>308</v>
+        <v>409</v>
       </c>
       <c r="K12" t="n">
-        <v>0.353802</v>
+        <v>0.234811</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Quercitin</t>
+          <t>D3</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-5.323</v>
+        <v>-5.271</v>
       </c>
       <c r="C13" t="n">
-        <v>-2.754</v>
+        <v>-2.633</v>
       </c>
       <c r="D13" t="n">
-        <v>6.6676</v>
+        <v>3.3748</v>
       </c>
       <c r="E13" t="n">
-        <v>-1638.590312</v>
+        <v>-1444.874262</v>
       </c>
       <c r="F13" t="n">
-        <v>-1.058</v>
+        <v>-1.061</v>
       </c>
       <c r="G13" t="n">
-        <v>381.893317</v>
+        <v>346.581779</v>
       </c>
       <c r="H13" t="n">
-        <v>426.986904</v>
+        <v>402.922143</v>
       </c>
       <c r="I13" t="n">
         <v>-0</v>
       </c>
       <c r="J13" t="n">
-        <v>419</v>
+        <v>359</v>
       </c>
       <c r="K13" t="n">
-        <v>0.193758</v>
+        <v>0.109098</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Rutin</t>
+          <t>DPAA</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-5.159</v>
+        <v>-4.862</v>
       </c>
       <c r="C14" t="n">
-        <v>-2.833</v>
+        <v>-2.735</v>
       </c>
       <c r="D14" t="n">
-        <v>6.3594</v>
+        <v>5.8789</v>
       </c>
       <c r="E14" t="n">
-        <v>-2710.037461</v>
+        <v>-3704.69389</v>
       </c>
       <c r="F14" t="n">
-        <v>-1.971</v>
+        <v>-0.6850000000000001</v>
       </c>
       <c r="G14" t="n">
-        <v>631.881213</v>
+        <v>389.939641</v>
       </c>
       <c r="H14" t="n">
-        <v>731.916619</v>
+        <v>426.054576</v>
       </c>
       <c r="I14" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="K14" t="n">
-        <v>0.255696</v>
+        <v>0.499187</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>DPACA</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-5.418</v>
+        <v>-5.095</v>
       </c>
       <c r="C15" t="n">
-        <v>-3.71</v>
+        <v>-3.249</v>
       </c>
       <c r="D15" t="n">
-        <v>14.832</v>
+        <v>7.7768</v>
       </c>
       <c r="E15" t="n">
-        <v>-1464.797419</v>
+        <v>-3796.874182</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.012</v>
+        <v>-0.8159999999999999</v>
       </c>
       <c r="G15" t="n">
-        <v>373.33181</v>
+        <v>412.305213</v>
       </c>
       <c r="H15" t="n">
-        <v>386.599372</v>
+        <v>452.543801</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="J15" t="n">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="K15" t="n">
-        <v>0.952597</v>
+        <v>0.533851</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>Phenothiazine1</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-5.396</v>
+        <v>-4.935</v>
       </c>
       <c r="C16" t="n">
-        <v>-3.71</v>
+        <v>-3.333</v>
       </c>
       <c r="D16" t="n">
-        <v>15.8432</v>
+        <v>9.0352</v>
       </c>
       <c r="E16" t="n">
-        <v>-1618.511711</v>
+        <v>-1351.57215</v>
       </c>
       <c r="F16" t="n">
-        <v>-1.097</v>
+        <v>-0.765</v>
       </c>
       <c r="G16" t="n">
-        <v>417.523898</v>
+        <v>330.452395</v>
       </c>
       <c r="H16" t="n">
-        <v>431.785193</v>
+        <v>349.95115</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="J16" t="n">
-        <v>540</v>
+        <v>343</v>
       </c>
       <c r="K16" t="n">
-        <v>0.7944870000000001</v>
+        <v>0.288586</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>Phenothiazine2</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-5.448</v>
+        <v>-4.818</v>
       </c>
       <c r="C17" t="n">
-        <v>-3.863</v>
+        <v>-2.806</v>
       </c>
       <c r="D17" t="n">
-        <v>13.091</v>
+        <v>7.2013</v>
       </c>
       <c r="E17" t="n">
-        <v>-1633.444146</v>
+        <v>-1259.394134</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.952</v>
+        <v>-0.631</v>
       </c>
       <c r="G17" t="n">
-        <v>393.928755</v>
+        <v>311.25871</v>
       </c>
       <c r="H17" t="n">
-        <v>413.254515</v>
+        <v>327.396927</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="J17" t="n">
-        <v>560</v>
+        <v>308</v>
       </c>
       <c r="K17" t="n">
-        <v>1.005572</v>
+        <v>0.353802</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Phenothiazine3</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-5.34</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-3.153</v>
+      </c>
+      <c r="D18" t="n">
+        <v>9.789300000000001</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-953.539237</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-0.765</v>
+      </c>
+      <c r="G18" t="n">
+        <v>310.115745</v>
+      </c>
+      <c r="H18" t="n">
+        <v>326.248824</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>332</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.479784</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Phenothiazine4</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>-4.991</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-3.206</v>
+      </c>
+      <c r="D19" t="n">
+        <v>9.4053</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-1032.044192</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-0.759</v>
+      </c>
+      <c r="G19" t="n">
+        <v>333.827291</v>
+      </c>
+      <c r="H19" t="n">
+        <v>358.719796</v>
+      </c>
+      <c r="I19" t="n">
+        <v>-0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>524</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.534846</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Quercitin</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-5.323</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-2.754</v>
+      </c>
+      <c r="D20" t="n">
+        <v>6.6676</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-1638.590312</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-1.058</v>
+      </c>
+      <c r="G20" t="n">
+        <v>381.893317</v>
+      </c>
+      <c r="H20" t="n">
+        <v>426.986904</v>
+      </c>
+      <c r="I20" t="n">
+        <v>-0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>419</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.193758</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Rutin</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-5.159</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-2.833</v>
+      </c>
+      <c r="D21" t="n">
+        <v>6.3594</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-2710.037461</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-1.971</v>
+      </c>
+      <c r="G21" t="n">
+        <v>631.881213</v>
+      </c>
+      <c r="H21" t="n">
+        <v>731.916619</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>466</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.255696</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-5.418</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-3.71</v>
+      </c>
+      <c r="D22" t="n">
+        <v>14.832</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-1464.797419</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-1.012</v>
+      </c>
+      <c r="G22" t="n">
+        <v>373.33181</v>
+      </c>
+      <c r="H22" t="n">
+        <v>386.599372</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>523</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.952597</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-5.396</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-3.71</v>
+      </c>
+      <c r="D23" t="n">
+        <v>15.8432</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-1618.511711</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-1.097</v>
+      </c>
+      <c r="G23" t="n">
+        <v>417.523898</v>
+      </c>
+      <c r="H23" t="n">
+        <v>431.785193</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>540</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.7944870000000001</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>T3</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>-5.448</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-3.863</v>
+      </c>
+      <c r="D24" t="n">
+        <v>13.091</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-1633.444146</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-0.952</v>
+      </c>
+      <c r="G24" t="n">
+        <v>393.928755</v>
+      </c>
+      <c r="H24" t="n">
+        <v>413.254515</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>560</v>
+      </c>
+      <c r="K24" t="n">
+        <v>1.005572</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>T4</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="B25" t="n">
         <v>-5.429</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C25" t="n">
         <v>-3.866</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D25" t="n">
         <v>13.7502</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E25" t="n">
         <v>-1787.160542</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F25" t="n">
         <v>-1.021</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G25" t="n">
         <v>441.173419</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H25" t="n">
         <v>457.649836</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I25" t="n">
         <v>-0</v>
       </c>
-      <c r="J18" t="n">
+      <c r="J25" t="n">
         <v>583</v>
       </c>
-      <c r="K18" t="n">
+      <c r="K25" t="n">
         <v>0.7942709999999999</v>
       </c>
     </row>

</xml_diff>